<commit_message>
data from circuit containing zener for Q2
</commit_message>
<xml_diff>
--- a/data_analysis/xlsx/DMP4065S_Polarity_Overvoltage_Protection.xlsx
+++ b/data_analysis/xlsx/DMP4065S_Polarity_Overvoltage_Protection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelperry/Documents/GitHub/circuit_protection/data_analysis/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74F6524-E468-874C-A44D-4CA7BBBAEA5C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DE72DD-6694-3F40-9F98-760DB3999A1E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{8AB7D094-8CEA-A04F-8AB1-5D165CB29E23}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="4" xr2:uid="{8AB7D094-8CEA-A04F-8AB1-5D165CB29E23}"/>
   </bookViews>
   <sheets>
     <sheet name="Vin 10V" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="9">
   <si>
     <t>Vin</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Iout</t>
   </si>
   <si>
-    <t>Va</t>
-  </si>
-  <si>
     <t>TQ1</t>
   </si>
   <si>
@@ -58,6 +55,12 @@
   </si>
   <si>
     <t>Tamb</t>
+  </si>
+  <si>
+    <t>Va*</t>
+  </si>
+  <si>
+    <t>* Keithley 177 drifted during data collection</t>
   </si>
 </sst>
 </file>
@@ -119,20 +122,75 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>35000</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>7800</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>93536</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0718A2A7-6162-644E-BF28-61188F778AFA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7429500" y="0"/>
+          <a:ext cx="9144000" cy="4563936"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>35000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>128536</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9631526F-1DB5-0F40-9109-A237C3E9C89E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{088332C0-63E7-F244-9659-9270B10FE14E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -155,7 +213,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7429500" y="35000"/>
-          <a:ext cx="9144000" cy="5256000"/>
+          <a:ext cx="9144000" cy="4563936"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -167,27 +225,27 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>35000</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>7800</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>93536</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{725ECA80-D01E-D840-860D-D168F14FCB50}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5C07A0A-D38D-EA46-B063-82D00346E6C8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -209,8 +267,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7429500" y="35000"/>
-          <a:ext cx="9144000" cy="5256000"/>
+          <a:off x="7429500" y="0"/>
+          <a:ext cx="9144000" cy="4563936"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -222,27 +280,27 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>35000</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>7800</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>93536</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8A9C54C-7DE3-E94F-9BF2-6339E9B4CFEA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70A33194-ECEF-5349-983C-B63481F36642}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -264,8 +322,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7429500" y="35000"/>
-          <a:ext cx="9144000" cy="5256000"/>
+          <a:off x="7429500" y="0"/>
+          <a:ext cx="9144000" cy="4563936"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -277,27 +335,27 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>35000</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>7800</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>93536</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4291C8FE-2F9E-874D-AFC2-1248C6FFED4C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B98CCF7B-A6EA-654C-BE3F-2AA26FA1A688}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -319,63 +377,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7429500" y="35000"/>
-          <a:ext cx="9144000" cy="5256000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>35000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>7800</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F321DC2A-6AE8-AA4A-B4A6-89396088B034}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7429500" y="35000"/>
-          <a:ext cx="9144000" cy="5256000"/>
+          <a:off x="7429500" y="0"/>
+          <a:ext cx="9144000" cy="4563936"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -684,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEB92E55-A1A0-824A-A494-BDE0D38B5030}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -706,397 +709,397 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>10.005000000000001</v>
+        <v>10.007999999999999</v>
       </c>
       <c r="B2">
         <v>1.04E-2</v>
       </c>
       <c r="C2">
-        <v>9.9779999999999998</v>
+        <v>10.003</v>
       </c>
       <c r="D2">
-        <v>1.0200000000000001E-2</v>
+        <v>0.01</v>
       </c>
       <c r="E2">
-        <v>10.005000000000001</v>
+        <v>10.007999999999999</v>
       </c>
       <c r="F2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H2">
-        <v>21.8</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>10.005000000000001</v>
+        <v>10.007999999999999</v>
       </c>
       <c r="B3">
         <v>2.0299999999999999E-2</v>
       </c>
       <c r="C3">
-        <v>9.9760000000000009</v>
+        <v>10.002000000000001</v>
       </c>
       <c r="D3">
-        <v>0.02</v>
+        <v>1.9800000000000002E-2</v>
       </c>
       <c r="E3">
-        <v>10.004</v>
+        <v>10.007999999999999</v>
       </c>
       <c r="F3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H3">
-        <v>21.9</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>10.005000000000001</v>
+        <v>10.007999999999999</v>
       </c>
       <c r="B4">
         <v>3.0599999999999999E-2</v>
       </c>
       <c r="C4">
-        <v>9.9740000000000002</v>
+        <v>10</v>
       </c>
       <c r="D4">
-        <v>3.04E-2</v>
+        <v>3.0200000000000001E-2</v>
       </c>
       <c r="E4">
-        <v>10.004</v>
+        <v>10.007</v>
       </c>
       <c r="F4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H4">
-        <v>21.9</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>10.005000000000001</v>
+        <v>10.007999999999999</v>
       </c>
       <c r="B5">
         <v>4.0399999999999998E-2</v>
       </c>
       <c r="C5">
-        <v>9.9730000000000008</v>
+        <v>9.9990000000000006</v>
       </c>
       <c r="D5">
-        <v>4.02E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E5">
-        <v>10.003</v>
+        <v>10.006</v>
       </c>
       <c r="F5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H5">
-        <v>21.9</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>10.005000000000001</v>
+        <v>10.007999999999999</v>
       </c>
       <c r="B6">
-        <v>5.0200000000000002E-2</v>
+        <v>5.0299999999999997E-2</v>
       </c>
       <c r="C6">
-        <v>9.9719999999999995</v>
+        <v>9.9979999999999993</v>
       </c>
       <c r="D6">
-        <v>0.05</v>
+        <v>4.9799999999999997E-2</v>
       </c>
       <c r="E6">
-        <v>10.003</v>
+        <v>10.006</v>
       </c>
       <c r="F6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H6">
-        <v>22</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
+        <v>10.007999999999999</v>
+      </c>
+      <c r="B7">
+        <v>6.0499999999999998E-2</v>
+      </c>
+      <c r="C7">
+        <v>9.9960000000000004</v>
+      </c>
+      <c r="D7">
+        <v>6.0100000000000001E-2</v>
+      </c>
+      <c r="E7">
         <v>10.005000000000001</v>
       </c>
-      <c r="B7">
-        <v>6.0600000000000001E-2</v>
-      </c>
-      <c r="C7">
-        <v>9.9700000000000006</v>
-      </c>
-      <c r="D7">
-        <v>6.0299999999999999E-2</v>
-      </c>
-      <c r="E7">
-        <v>10.002000000000001</v>
-      </c>
       <c r="F7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H7">
-        <v>22</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>10.005000000000001</v>
+        <v>10.007999999999999</v>
       </c>
       <c r="B8">
         <v>7.0400000000000004E-2</v>
       </c>
       <c r="C8">
-        <v>9.9689999999999994</v>
+        <v>9.9949999999999992</v>
       </c>
       <c r="D8">
-        <v>7.0099999999999996E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E8">
-        <v>10.002000000000001</v>
+        <v>10.004</v>
       </c>
       <c r="F8">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G8">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H8">
-        <v>22</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>10.005000000000001</v>
+        <v>10.007999999999999</v>
       </c>
       <c r="B9">
-        <v>8.0299999999999996E-2</v>
+        <v>8.0199999999999994E-2</v>
       </c>
       <c r="C9">
-        <v>9.9670000000000005</v>
+        <v>9.9930000000000003</v>
       </c>
       <c r="D9">
-        <v>0.08</v>
+        <v>7.9799999999999996E-2</v>
       </c>
       <c r="E9">
-        <v>10.000999999999999</v>
+        <v>10.004</v>
       </c>
       <c r="F9">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G9">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H9">
-        <v>22</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>10.005000000000001</v>
+        <v>10.007999999999999</v>
       </c>
       <c r="B10">
         <v>9.06E-2</v>
       </c>
       <c r="C10">
-        <v>9.9659999999999993</v>
+        <v>9.9920000000000009</v>
       </c>
       <c r="D10">
-        <v>9.0300000000000005E-2</v>
+        <v>9.01E-2</v>
       </c>
       <c r="E10">
-        <v>10.000999999999999</v>
+        <v>10.003</v>
       </c>
       <c r="F10">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G10">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H10">
-        <v>22.1</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>10.005000000000001</v>
+        <v>10.007999999999999</v>
       </c>
       <c r="B11">
         <v>0.1004</v>
       </c>
       <c r="C11">
-        <v>9.9640000000000004</v>
+        <v>9.99</v>
       </c>
       <c r="D11">
-        <v>0.10009999999999999</v>
+        <v>9.9900000000000003E-2</v>
       </c>
       <c r="E11">
-        <v>10</v>
+        <v>10.002000000000001</v>
       </c>
       <c r="F11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H11">
-        <v>22.1</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>10.005000000000001</v>
+        <v>10.007</v>
       </c>
       <c r="B12">
-        <v>0.20069999999999999</v>
+        <v>0.2006</v>
       </c>
       <c r="C12">
-        <v>9.9499999999999993</v>
+        <v>9.9760000000000009</v>
       </c>
       <c r="D12">
-        <v>0.20030000000000001</v>
+        <v>0.2001</v>
       </c>
       <c r="E12">
-        <v>9.9930000000000003</v>
+        <v>9.9960000000000004</v>
       </c>
       <c r="F12">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G12">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H12">
-        <v>22.1</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>10.005000000000001</v>
+        <v>10.007</v>
       </c>
       <c r="B13">
         <v>0.3009</v>
       </c>
       <c r="C13">
-        <v>9.9350000000000005</v>
+        <v>9.9610000000000003</v>
       </c>
       <c r="D13">
-        <v>0.30030000000000001</v>
+        <v>0.30009999999999998</v>
       </c>
       <c r="E13">
-        <v>9.9870000000000001</v>
+        <v>9.99</v>
       </c>
       <c r="F13">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G13">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H13">
-        <v>22.1</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>10.005000000000001</v>
+        <v>10.007</v>
       </c>
       <c r="B14">
         <v>0.40060000000000001</v>
       </c>
       <c r="C14">
-        <v>9.92</v>
+        <v>9.9469999999999992</v>
       </c>
       <c r="D14">
-        <v>0.39989999999999998</v>
+        <v>0.3997</v>
       </c>
       <c r="E14">
-        <v>9.9809999999999999</v>
+        <v>9.9830000000000005</v>
       </c>
       <c r="F14">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G14">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H14">
-        <v>22.1</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>10.005000000000001</v>
+        <v>10.007</v>
       </c>
       <c r="B15">
-        <v>0.50090000000000001</v>
+        <v>0.50080000000000002</v>
       </c>
       <c r="C15">
-        <v>9.9049999999999994</v>
+        <v>9.9320000000000004</v>
       </c>
       <c r="D15">
-        <v>0.5</v>
+        <v>0.49980000000000002</v>
       </c>
       <c r="E15">
-        <v>9.9749999999999996</v>
+        <v>9.9770000000000003</v>
       </c>
       <c r="F15">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G15">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H15">
-        <v>22.1</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>10.005000000000001</v>
+        <v>10.007</v>
       </c>
       <c r="B16">
-        <v>0.60109999999999997</v>
+        <v>0.60099999999999998</v>
       </c>
       <c r="C16">
-        <v>9.89</v>
+        <v>9.9169999999999998</v>
       </c>
       <c r="D16">
-        <v>0.60019999999999996</v>
+        <v>0.6</v>
       </c>
       <c r="E16">
-        <v>9.968</v>
+        <v>9.9700000000000006</v>
       </c>
       <c r="F16">
         <v>23</v>
@@ -1105,371 +1108,374 @@
         <v>23</v>
       </c>
       <c r="H16">
-        <v>22.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>10.005000000000001</v>
+        <v>10.007</v>
       </c>
       <c r="B17">
-        <v>0.70130000000000003</v>
+        <v>0.70120000000000005</v>
       </c>
       <c r="C17">
-        <v>9.875</v>
+        <v>9.9009999999999998</v>
       </c>
       <c r="D17">
-        <v>0.70040000000000002</v>
+        <v>0.70020000000000004</v>
       </c>
       <c r="E17">
-        <v>9.9619999999999997</v>
+        <v>9.9640000000000004</v>
       </c>
       <c r="F17">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G17">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H17">
-        <v>22.1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>10.005000000000001</v>
+        <v>10.007</v>
       </c>
       <c r="B18">
-        <v>0.80110000000000003</v>
+        <v>0.80100000000000005</v>
       </c>
       <c r="C18">
-        <v>9.859</v>
+        <v>9.8859999999999992</v>
       </c>
       <c r="D18">
-        <v>0.79979999999999996</v>
+        <v>0.79949999999999999</v>
       </c>
       <c r="E18">
-        <v>9.9550000000000001</v>
+        <v>9.9570000000000007</v>
       </c>
       <c r="F18">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G18">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H18">
-        <v>22.1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>10.004</v>
+        <v>10.007</v>
       </c>
       <c r="B19">
-        <v>0.90129999999999999</v>
+        <v>0.9012</v>
       </c>
       <c r="C19">
-        <v>9.843</v>
+        <v>9.8699999999999992</v>
       </c>
       <c r="D19">
-        <v>0.89990000000000003</v>
+        <v>0.89970000000000006</v>
       </c>
       <c r="E19">
-        <v>9.9480000000000004</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="F19">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G19">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H19">
-        <v>22.1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>10.004</v>
+        <v>10.007</v>
       </c>
       <c r="B20">
         <v>1.0015000000000001</v>
       </c>
       <c r="C20">
-        <v>9.827</v>
+        <v>9.8539999999999992</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0.99980000000000002</v>
       </c>
       <c r="E20">
-        <v>9.9410000000000007</v>
+        <v>9.9420000000000002</v>
       </c>
       <c r="F20">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G20">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H20">
-        <v>22.1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>10.004</v>
+        <v>10.006</v>
       </c>
       <c r="B21">
         <v>1.1016999999999999</v>
       </c>
       <c r="C21">
-        <v>9.81</v>
+        <v>9.8369999999999997</v>
       </c>
       <c r="D21">
-        <v>1.1002000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E21">
-        <v>9.9339999999999993</v>
+        <v>9.9350000000000005</v>
       </c>
       <c r="F21">
         <v>28</v>
       </c>
       <c r="G21">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H21">
-        <v>22.1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>10.004</v>
+        <v>10.006</v>
       </c>
       <c r="B22">
-        <v>1.2015</v>
+        <v>1.2014</v>
       </c>
       <c r="C22">
-        <v>9.7929999999999993</v>
+        <v>9.8190000000000008</v>
       </c>
       <c r="D22">
-        <v>1.1999</v>
+        <v>1.1997</v>
       </c>
       <c r="E22">
-        <v>9.9250000000000007</v>
+        <v>9.9280000000000008</v>
       </c>
       <c r="F22">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G22">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H22">
-        <v>22.1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>10.004</v>
+        <v>10.006</v>
       </c>
       <c r="B23">
-        <v>1.3018000000000001</v>
+        <v>1.3016000000000001</v>
       </c>
       <c r="C23">
-        <v>9.7739999999999991</v>
+        <v>9.8019999999999996</v>
       </c>
       <c r="D23">
-        <v>1.2999000000000001</v>
+        <v>1.2997000000000001</v>
       </c>
       <c r="E23">
-        <v>9.9179999999999993</v>
+        <v>9.92</v>
       </c>
       <c r="F23">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G23">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H23">
-        <v>22.1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>10.004</v>
+        <v>10.006</v>
       </c>
       <c r="B24">
-        <v>1.4019999999999999</v>
+        <v>1.4018999999999999</v>
       </c>
       <c r="C24">
-        <v>9.7560000000000002</v>
+        <v>9.7829999999999995</v>
       </c>
       <c r="D24">
-        <v>1.4000999999999999</v>
+        <v>1.3997999999999999</v>
       </c>
       <c r="E24">
-        <v>9.91</v>
+        <v>9.9120000000000008</v>
       </c>
       <c r="F24">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G24">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H24">
-        <v>22.1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23.1</v>
+      </c>
+      <c r="J24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>10.004</v>
+        <v>10.006</v>
       </c>
       <c r="B25">
-        <v>1.5023</v>
+        <v>1.5021</v>
       </c>
       <c r="C25">
-        <v>9.7349999999999994</v>
+        <v>9.7639999999999993</v>
       </c>
       <c r="D25">
-        <v>1.5002</v>
+        <v>1.5</v>
       </c>
       <c r="E25">
-        <v>9.9009999999999998</v>
+        <v>9.9039999999999999</v>
       </c>
       <c r="F25">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G25">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H25">
-        <v>22.1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>10.004</v>
+        <v>10.006</v>
       </c>
       <c r="B26">
-        <v>1.6020000000000001</v>
+        <v>1.6017999999999999</v>
       </c>
       <c r="C26">
-        <v>9.7140000000000004</v>
+        <v>9.7439999999999998</v>
       </c>
       <c r="D26">
-        <v>1.5999000000000001</v>
+        <v>1.5996999999999999</v>
       </c>
       <c r="E26">
-        <v>9.8919999999999995</v>
+        <v>10.022</v>
       </c>
       <c r="F26">
         <v>36</v>
       </c>
       <c r="G26">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H26">
-        <v>22.1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>10.003</v>
+        <v>10.006</v>
       </c>
       <c r="B27">
-        <v>1.7023999999999999</v>
+        <v>1.7021999999999999</v>
       </c>
       <c r="C27">
-        <v>9.6929999999999996</v>
+        <v>9.7219999999999995</v>
       </c>
       <c r="D27">
-        <v>1.7001999999999999</v>
+        <v>1.7</v>
       </c>
       <c r="E27">
-        <v>9.8829999999999991</v>
+        <v>10.013</v>
       </c>
       <c r="F27">
         <v>38</v>
       </c>
       <c r="G27">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H27">
-        <v>22.1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>10.003</v>
+        <v>10.006</v>
       </c>
       <c r="B28">
-        <v>1.8026</v>
+        <v>1.8024</v>
       </c>
       <c r="C28">
-        <v>9.67</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="D28">
-        <v>1.8003</v>
+        <v>1.8001</v>
       </c>
       <c r="E28">
-        <v>9.8719999999999999</v>
+        <v>10.002000000000001</v>
       </c>
       <c r="F28">
         <v>41</v>
       </c>
       <c r="G28">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H28">
-        <v>22.1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>10.003</v>
+        <v>10.006</v>
       </c>
       <c r="B29">
-        <v>1.9029</v>
+        <v>1.9026000000000001</v>
       </c>
       <c r="C29">
-        <v>9.6460000000000008</v>
+        <v>9.6750000000000007</v>
       </c>
       <c r="D29">
-        <v>1.9005000000000001</v>
+        <v>1.9001999999999999</v>
       </c>
       <c r="E29">
-        <v>9.8620000000000001</v>
+        <v>9.9920000000000009</v>
       </c>
       <c r="F29">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G29">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="H29">
-        <v>22.1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>10.003</v>
+        <v>10.005000000000001</v>
       </c>
       <c r="B30">
-        <v>2.0026000000000002</v>
+        <v>2.0023</v>
       </c>
       <c r="C30">
-        <v>9.6189999999999998</v>
+        <v>9.65</v>
       </c>
       <c r="D30">
-        <v>2.0009999999999999</v>
+        <v>1.9998</v>
       </c>
       <c r="E30">
-        <v>9.85</v>
+        <v>9.98</v>
       </c>
       <c r="F30">
         <v>47</v>
       </c>
       <c r="G30">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H30">
-        <v>22.1</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1480,7 +1486,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96723608-9729-B847-9516-F7512128F7D0}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
@@ -1488,7 +1494,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1510,762 +1516,672 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>12.073</v>
+        <v>12.013999999999999</v>
       </c>
       <c r="B2">
-        <v>1.06E-2</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="C2">
-        <v>12.035</v>
+        <v>12.013</v>
       </c>
       <c r="D2">
-        <v>1.0200000000000001E-2</v>
+        <v>0.01</v>
       </c>
       <c r="E2">
-        <v>12.074999999999999</v>
+        <v>22</v>
       </c>
       <c r="F2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2">
-        <v>21</v>
-      </c>
-      <c r="H2">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>12.073</v>
+        <v>12.013999999999999</v>
       </c>
       <c r="B3">
-        <v>2.0400000000000001E-2</v>
+        <v>2.0299999999999999E-2</v>
       </c>
       <c r="C3">
-        <v>12.032999999999999</v>
+        <v>12.010999999999999</v>
       </c>
       <c r="D3">
-        <v>0.02</v>
+        <v>1.9800000000000002E-2</v>
       </c>
       <c r="E3">
-        <v>12.074</v>
+        <v>22</v>
       </c>
       <c r="F3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3">
-        <v>21</v>
-      </c>
-      <c r="H3">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>12.073</v>
+        <v>12.013999999999999</v>
       </c>
       <c r="B4">
-        <v>3.0800000000000001E-2</v>
+        <v>3.0599999999999999E-2</v>
       </c>
       <c r="C4">
-        <v>12.032</v>
+        <v>12.01</v>
       </c>
       <c r="D4">
-        <v>3.04E-2</v>
+        <v>3.0200000000000001E-2</v>
       </c>
       <c r="E4">
-        <v>12.073</v>
+        <v>22</v>
       </c>
       <c r="F4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G4">
-        <v>21</v>
-      </c>
-      <c r="H4">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>12.073</v>
+        <v>12.013999999999999</v>
       </c>
       <c r="B5">
-        <v>4.0599999999999997E-2</v>
+        <v>4.0500000000000001E-2</v>
       </c>
       <c r="C5">
-        <v>12.031000000000001</v>
+        <v>12.009</v>
       </c>
       <c r="D5">
-        <v>4.02E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E5">
-        <v>12.073</v>
+        <v>22</v>
       </c>
       <c r="F5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G5">
-        <v>21</v>
-      </c>
-      <c r="H5">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>12.073</v>
+        <v>12.013999999999999</v>
       </c>
       <c r="B6">
-        <v>5.04E-2</v>
+        <v>5.0299999999999997E-2</v>
       </c>
       <c r="C6">
-        <v>12.029</v>
+        <v>12.007</v>
       </c>
       <c r="D6">
-        <v>0.05</v>
+        <v>4.9799999999999997E-2</v>
       </c>
       <c r="E6">
-        <v>12.071999999999999</v>
+        <v>22</v>
       </c>
       <c r="F6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G6">
-        <v>21</v>
-      </c>
-      <c r="H6">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>12.073</v>
+        <v>12.013999999999999</v>
       </c>
       <c r="B7">
-        <v>6.08E-2</v>
+        <v>6.0600000000000001E-2</v>
       </c>
       <c r="C7">
-        <v>12.028</v>
+        <v>12.006</v>
       </c>
       <c r="D7">
-        <v>6.0299999999999999E-2</v>
+        <v>6.0100000000000001E-2</v>
       </c>
       <c r="E7">
-        <v>12.071</v>
+        <v>22</v>
       </c>
       <c r="F7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G7">
-        <v>21</v>
-      </c>
-      <c r="H7">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>12.073</v>
+        <v>12.013999999999999</v>
       </c>
       <c r="B8">
-        <v>7.0599999999999996E-2</v>
+        <v>7.0400000000000004E-2</v>
       </c>
       <c r="C8">
-        <v>12.026</v>
+        <v>12.004</v>
       </c>
       <c r="D8">
-        <v>7.0099999999999996E-2</v>
+        <v>6.9900000000000004E-2</v>
       </c>
       <c r="E8">
-        <v>12.07</v>
+        <v>22</v>
       </c>
       <c r="F8">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G8">
-        <v>21</v>
-      </c>
-      <c r="H8">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>12.073</v>
+        <v>12.013999999999999</v>
       </c>
       <c r="B9">
-        <v>8.0399999999999999E-2</v>
+        <v>8.0199999999999994E-2</v>
       </c>
       <c r="C9">
-        <v>12.025</v>
+        <v>12.003</v>
       </c>
       <c r="D9">
-        <v>0.08</v>
+        <v>7.9799999999999996E-2</v>
       </c>
       <c r="E9">
-        <v>12.07</v>
+        <v>22</v>
       </c>
       <c r="F9">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G9">
-        <v>21</v>
-      </c>
-      <c r="H9">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>12.073</v>
+        <v>12.013999999999999</v>
       </c>
       <c r="B10">
-        <v>9.0700000000000003E-2</v>
+        <v>9.0499999999999997E-2</v>
       </c>
       <c r="C10">
-        <v>12.023</v>
+        <v>12.000999999999999</v>
       </c>
       <c r="D10">
-        <v>9.0300000000000005E-2</v>
+        <v>9.01E-2</v>
       </c>
       <c r="E10">
-        <v>12.07</v>
+        <v>22</v>
       </c>
       <c r="F10">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G10">
-        <v>21</v>
-      </c>
-      <c r="H10">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>12.073</v>
+        <v>12.013999999999999</v>
       </c>
       <c r="B11">
-        <v>0.10059999999999999</v>
+        <v>0.1003</v>
       </c>
       <c r="C11">
-        <v>12.022</v>
+        <v>12</v>
       </c>
       <c r="D11">
-        <v>0.10009999999999999</v>
+        <v>9.9900000000000003E-2</v>
       </c>
       <c r="E11">
-        <v>12.069000000000001</v>
+        <v>22</v>
       </c>
       <c r="F11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G11">
-        <v>21</v>
-      </c>
-      <c r="H11">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>12.071999999999999</v>
+        <v>12.013999999999999</v>
       </c>
       <c r="B12">
-        <v>0.20080000000000001</v>
+        <v>0.2006</v>
       </c>
       <c r="C12">
-        <v>12.007999999999999</v>
+        <v>11.986000000000001</v>
       </c>
       <c r="D12">
-        <v>0.20030000000000001</v>
+        <v>0.2001</v>
       </c>
       <c r="E12">
-        <v>12.063000000000001</v>
+        <v>22</v>
       </c>
       <c r="F12">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G12">
-        <v>21</v>
-      </c>
-      <c r="H12">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>12.071999999999999</v>
+        <v>12.013999999999999</v>
       </c>
       <c r="B13">
-        <v>0.30099999999999999</v>
+        <v>0.3009</v>
       </c>
       <c r="C13">
-        <v>11.994</v>
+        <v>11.971</v>
       </c>
       <c r="D13">
-        <v>0.30030000000000001</v>
+        <v>0.30009999999999998</v>
       </c>
       <c r="E13">
-        <v>12.055999999999999</v>
+        <v>22</v>
       </c>
       <c r="F13">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G13">
-        <v>21</v>
-      </c>
-      <c r="H13">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>12.071999999999999</v>
+        <v>12.013999999999999</v>
       </c>
       <c r="B14">
-        <v>0.4007</v>
+        <v>0.40060000000000001</v>
       </c>
       <c r="C14">
-        <v>11.978999999999999</v>
+        <v>11.957000000000001</v>
       </c>
       <c r="D14">
-        <v>0.39989999999999998</v>
+        <v>0.3997</v>
       </c>
       <c r="E14">
-        <v>12.051</v>
+        <v>23</v>
       </c>
       <c r="F14">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G14">
-        <v>21</v>
-      </c>
-      <c r="H14">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>12.071999999999999</v>
+        <v>12.013999999999999</v>
       </c>
       <c r="B15">
-        <v>0.501</v>
+        <v>0.50080000000000002</v>
       </c>
       <c r="C15">
-        <v>11.965</v>
+        <v>11.943</v>
       </c>
       <c r="D15">
-        <v>0.50009999999999999</v>
+        <v>0.49980000000000002</v>
       </c>
       <c r="E15">
-        <v>12.045</v>
+        <v>23</v>
       </c>
       <c r="F15">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G15">
-        <v>21</v>
-      </c>
-      <c r="H15">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>12.071999999999999</v>
+        <v>12.013999999999999</v>
       </c>
       <c r="B16">
-        <v>0.60119999999999996</v>
+        <v>0.60109999999999997</v>
       </c>
       <c r="C16">
-        <v>11.95</v>
+        <v>11.928000000000001</v>
       </c>
       <c r="D16">
-        <v>0.60019999999999996</v>
+        <v>0.6</v>
       </c>
       <c r="E16">
-        <v>12.038</v>
+        <v>23</v>
       </c>
       <c r="F16">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G16">
-        <v>22</v>
-      </c>
-      <c r="H16">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>12.071999999999999</v>
+        <v>12.013999999999999</v>
       </c>
       <c r="B17">
-        <v>0.70140000000000002</v>
+        <v>0.70120000000000005</v>
       </c>
       <c r="C17">
-        <v>11.935</v>
+        <v>11.913</v>
       </c>
       <c r="D17">
-        <v>0.70040000000000002</v>
+        <v>0.70020000000000004</v>
       </c>
       <c r="E17">
-        <v>12.032</v>
+        <v>24</v>
       </c>
       <c r="F17">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G17">
-        <v>23</v>
-      </c>
-      <c r="H17">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>12.071999999999999</v>
+        <v>12.013</v>
       </c>
       <c r="B18">
-        <v>0.80120000000000002</v>
+        <v>0.80100000000000005</v>
       </c>
       <c r="C18">
-        <v>11.92</v>
+        <v>11.898</v>
       </c>
       <c r="D18">
-        <v>0.79979999999999996</v>
+        <v>0.79959999999999998</v>
       </c>
       <c r="E18">
-        <v>12.026</v>
+        <v>24</v>
       </c>
       <c r="F18">
         <v>24</v>
       </c>
       <c r="G18">
-        <v>23</v>
-      </c>
-      <c r="H18">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>12.071999999999999</v>
+        <v>12.013</v>
       </c>
       <c r="B19">
-        <v>0.90139999999999998</v>
+        <v>0.9012</v>
       </c>
       <c r="C19">
-        <v>11.904999999999999</v>
+        <v>11.882</v>
       </c>
       <c r="D19">
-        <v>0.89990000000000003</v>
+        <v>0.89970000000000006</v>
       </c>
       <c r="E19">
-        <v>12.019</v>
+        <v>26</v>
       </c>
       <c r="F19">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G19">
-        <v>24</v>
-      </c>
-      <c r="H19">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>12.071999999999999</v>
+        <v>12.013</v>
       </c>
       <c r="B20">
-        <v>1.0017</v>
+        <v>1.0015000000000001</v>
       </c>
       <c r="C20">
-        <v>11.888999999999999</v>
+        <v>11.866</v>
       </c>
       <c r="D20">
-        <v>1.0001</v>
+        <v>0.99990000000000001</v>
       </c>
       <c r="E20">
-        <v>12.012</v>
+        <v>26</v>
       </c>
       <c r="F20">
         <v>26</v>
       </c>
       <c r="G20">
-        <v>25</v>
-      </c>
-      <c r="H20">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>12.071999999999999</v>
+        <v>12.013</v>
       </c>
       <c r="B21">
-        <v>1.1019000000000001</v>
+        <v>1.1016999999999999</v>
       </c>
       <c r="C21">
-        <v>11.872</v>
+        <v>11.85</v>
       </c>
       <c r="D21">
-        <v>1.1003000000000001</v>
+        <v>1.1001000000000001</v>
       </c>
       <c r="E21">
-        <v>12.005000000000001</v>
+        <v>28</v>
       </c>
       <c r="F21">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G21">
-        <v>26</v>
-      </c>
-      <c r="H21">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>12.071</v>
+        <v>12.013</v>
       </c>
       <c r="B22">
-        <v>1.2016</v>
+        <v>1.2014</v>
       </c>
       <c r="C22">
-        <v>11.856</v>
+        <v>11.833</v>
       </c>
       <c r="D22">
-        <v>1.1999</v>
+        <v>1.1997</v>
       </c>
       <c r="E22">
-        <v>11.997</v>
+        <v>29</v>
       </c>
       <c r="F22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G22">
-        <v>27</v>
-      </c>
-      <c r="H22">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>12.071</v>
+        <v>12.013</v>
       </c>
       <c r="B23">
-        <v>1.3018000000000001</v>
+        <v>1.3017000000000001</v>
       </c>
       <c r="C23">
-        <v>11.837</v>
+        <v>11.816000000000001</v>
       </c>
       <c r="D23">
-        <v>1.2999000000000001</v>
+        <v>1.2997000000000001</v>
       </c>
       <c r="E23">
-        <v>11.99</v>
+        <v>31</v>
       </c>
       <c r="F23">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G23">
-        <v>29</v>
-      </c>
-      <c r="H23">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>12.071</v>
+        <v>12.013</v>
       </c>
       <c r="B24">
-        <v>1.4020999999999999</v>
+        <v>1.4018999999999999</v>
       </c>
       <c r="C24">
-        <v>11.819000000000001</v>
+        <v>11.797000000000001</v>
       </c>
       <c r="D24">
-        <v>1.4000999999999999</v>
+        <v>1.3997999999999999</v>
       </c>
       <c r="E24">
-        <v>11.981999999999999</v>
+        <v>33</v>
       </c>
       <c r="F24">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G24">
-        <v>30</v>
-      </c>
-      <c r="H24">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>12.071</v>
+        <v>12.013</v>
       </c>
       <c r="B25">
-        <v>1.5018</v>
+        <v>1.5021</v>
       </c>
       <c r="C25">
-        <v>11.824</v>
+        <v>11.778</v>
       </c>
       <c r="D25">
-        <v>1.5001</v>
+        <v>1.5</v>
       </c>
       <c r="E25">
-        <v>11.973000000000001</v>
+        <v>34</v>
       </c>
       <c r="F25">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G25">
-        <v>32</v>
-      </c>
-      <c r="H25">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>12.071</v>
+        <v>12.012</v>
       </c>
       <c r="B26">
-        <v>1.6015999999999999</v>
+        <v>1.6019000000000001</v>
       </c>
       <c r="C26">
-        <v>11.811</v>
+        <v>11.757999999999999</v>
       </c>
       <c r="D26">
-        <v>1.5996999999999999</v>
+        <v>1.5995999999999999</v>
       </c>
       <c r="E26">
-        <v>11.965</v>
+        <v>36</v>
       </c>
       <c r="F26">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G26">
-        <v>33</v>
-      </c>
-      <c r="H26">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>12.071</v>
+        <v>12.012</v>
       </c>
       <c r="B27">
-        <v>1.702</v>
+        <v>1.7021999999999999</v>
       </c>
       <c r="C27">
-        <v>11.792999999999999</v>
+        <v>11.737</v>
       </c>
       <c r="D27">
-        <v>1.7</v>
+        <v>1.6999</v>
       </c>
       <c r="E27">
-        <v>11.956</v>
+        <v>39</v>
       </c>
       <c r="F27">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G27">
-        <v>35</v>
-      </c>
-      <c r="H27">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>12.071</v>
+        <v>12.012</v>
       </c>
       <c r="B28">
-        <v>1.8022</v>
+        <v>1.8025</v>
       </c>
       <c r="C28">
-        <v>11.772</v>
+        <v>11.715</v>
       </c>
       <c r="D28">
         <v>1.8001</v>
       </c>
       <c r="E28">
-        <v>11.946</v>
+        <v>41</v>
       </c>
       <c r="F28">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G28">
-        <v>38</v>
-      </c>
-      <c r="H28">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>12.071</v>
+        <v>12.012</v>
       </c>
       <c r="B29">
-        <v>1.9025000000000001</v>
+        <v>1.9026000000000001</v>
       </c>
       <c r="C29">
-        <v>11.749000000000001</v>
+        <v>11.693</v>
       </c>
       <c r="D29">
         <v>1.9003000000000001</v>
       </c>
       <c r="E29">
-        <v>11.936</v>
+        <v>44</v>
       </c>
       <c r="F29">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G29">
-        <v>40</v>
-      </c>
-      <c r="H29">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>12.071</v>
+        <v>12.012</v>
       </c>
       <c r="B30">
-        <v>2.0022000000000002</v>
+        <v>2.0023</v>
       </c>
       <c r="C30">
-        <v>11.726000000000001</v>
+        <v>11.667999999999999</v>
       </c>
       <c r="D30">
-        <v>1.9998</v>
+        <v>1.9999</v>
       </c>
       <c r="E30">
-        <v>11.926</v>
+        <v>47</v>
       </c>
       <c r="F30">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G30">
-        <v>43</v>
-      </c>
-      <c r="H30">
-        <v>22.2</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2276,7 +2192,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130CBAC5-66D5-294E-9A62-E40DF8B7ED0F}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
@@ -2284,7 +2200,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2306,172 +2222,151 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>16.024999999999999</v>
       </c>
       <c r="B2">
-        <v>1.06E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="C2">
         <v>16.021000000000001</v>
       </c>
       <c r="D2">
-        <v>0.01</v>
+        <v>1.01E-2</v>
       </c>
       <c r="E2">
-        <v>16.027000000000001</v>
+        <v>22</v>
       </c>
       <c r="F2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2">
-        <v>21</v>
-      </c>
-      <c r="H2">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>16.024999999999999</v>
       </c>
       <c r="B3">
-        <v>2.0500000000000001E-2</v>
+        <v>2.0799999999999999E-2</v>
       </c>
       <c r="C3">
         <v>16.02</v>
       </c>
       <c r="D3">
-        <v>1.9800000000000002E-2</v>
+        <v>1.9900000000000001E-2</v>
       </c>
       <c r="E3">
-        <v>16.027000000000001</v>
+        <v>22</v>
       </c>
       <c r="F3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3">
-        <v>21</v>
-      </c>
-      <c r="H3">
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>16.024999999999999</v>
       </c>
       <c r="B4">
-        <v>3.0800000000000001E-2</v>
+        <v>3.1199999999999999E-2</v>
       </c>
       <c r="C4">
-        <v>16.018000000000001</v>
+        <v>16.018999999999998</v>
       </c>
       <c r="D4">
         <v>3.0200000000000001E-2</v>
       </c>
       <c r="E4">
-        <v>16.026</v>
+        <v>22</v>
       </c>
       <c r="F4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G4">
-        <v>21</v>
-      </c>
-      <c r="H4">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>16.024999999999999</v>
+        <v>16.016999999999999</v>
       </c>
       <c r="B5">
-        <v>4.0599999999999997E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="C5">
         <v>16.016999999999999</v>
       </c>
       <c r="D5">
-        <v>0.04</v>
+        <v>4.0099999999999997E-2</v>
       </c>
       <c r="E5">
-        <v>16.026</v>
+        <v>22</v>
       </c>
       <c r="F5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G5">
-        <v>21</v>
-      </c>
-      <c r="H5">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>16.024999999999999</v>
       </c>
       <c r="B6">
-        <v>5.0500000000000003E-2</v>
+        <v>5.0799999999999998E-2</v>
       </c>
       <c r="C6">
         <v>16.015999999999998</v>
       </c>
       <c r="D6">
-        <v>4.9799999999999997E-2</v>
+        <v>4.99E-2</v>
       </c>
       <c r="E6">
-        <v>16.024999999999999</v>
+        <v>22</v>
       </c>
       <c r="F6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G6">
-        <v>21</v>
-      </c>
-      <c r="H6">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>16.024999999999999</v>
       </c>
       <c r="B7">
-        <v>6.08E-2</v>
+        <v>6.1100000000000002E-2</v>
       </c>
       <c r="C7">
         <v>16.013999999999999</v>
       </c>
       <c r="D7">
-        <v>6.0100000000000001E-2</v>
+        <v>6.0199999999999997E-2</v>
       </c>
       <c r="E7">
-        <v>16.024000000000001</v>
+        <v>22</v>
       </c>
       <c r="F7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G7">
-        <v>21</v>
-      </c>
-      <c r="H7">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>16.024999999999999</v>
       </c>
       <c r="B8">
-        <v>7.0599999999999996E-2</v>
+        <v>7.0900000000000005E-2</v>
       </c>
       <c r="C8">
         <v>16.013000000000002</v>
@@ -2480,24 +2375,21 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E8">
-        <v>16.023</v>
+        <v>22</v>
       </c>
       <c r="F8">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G8">
-        <v>21</v>
-      </c>
-      <c r="H8">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>16.024999999999999</v>
       </c>
       <c r="B9">
-        <v>8.0399999999999999E-2</v>
+        <v>8.0799999999999997E-2</v>
       </c>
       <c r="C9">
         <v>16.012</v>
@@ -2506,24 +2398,21 @@
         <v>7.9799999999999996E-2</v>
       </c>
       <c r="E9">
-        <v>16.023</v>
+        <v>22</v>
       </c>
       <c r="F9">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G9">
-        <v>21</v>
-      </c>
-      <c r="H9">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>16.024999999999999</v>
       </c>
       <c r="B10">
-        <v>9.0800000000000006E-2</v>
+        <v>9.11E-2</v>
       </c>
       <c r="C10">
         <v>16.010000000000002</v>
@@ -2532,24 +2421,21 @@
         <v>9.01E-2</v>
       </c>
       <c r="E10">
-        <v>16.023</v>
+        <v>22</v>
       </c>
       <c r="F10">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G10">
-        <v>21</v>
-      </c>
-      <c r="H10">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>16.024999999999999</v>
       </c>
       <c r="B11">
-        <v>0.10050000000000001</v>
+        <v>0.1009</v>
       </c>
       <c r="C11">
         <v>16.009</v>
@@ -2558,24 +2444,21 @@
         <v>9.9900000000000003E-2</v>
       </c>
       <c r="E11">
-        <v>16.021999999999998</v>
+        <v>22</v>
       </c>
       <c r="F11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G11">
-        <v>21</v>
-      </c>
-      <c r="H11">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>16.024999999999999</v>
       </c>
       <c r="B12">
-        <v>0.20080000000000001</v>
+        <v>0.20119999999999999</v>
       </c>
       <c r="C12">
         <v>15.994999999999999</v>
@@ -2584,128 +2467,113 @@
         <v>0.2001</v>
       </c>
       <c r="E12">
-        <v>16.015999999999998</v>
+        <v>22</v>
       </c>
       <c r="F12">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G12">
-        <v>21</v>
-      </c>
-      <c r="H12">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>16.024999999999999</v>
       </c>
       <c r="B13">
-        <v>0.30109999999999998</v>
+        <v>0.3014</v>
       </c>
       <c r="C13">
-        <v>15.981999999999999</v>
+        <v>15.981</v>
       </c>
       <c r="D13">
         <v>0.30009999999999998</v>
       </c>
       <c r="E13">
-        <v>16.010000000000002</v>
+        <v>22</v>
       </c>
       <c r="F13">
         <v>22</v>
       </c>
       <c r="G13">
-        <v>21</v>
-      </c>
-      <c r="H13">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>16.024999999999999</v>
+        <v>16.024000000000001</v>
       </c>
       <c r="B14">
-        <v>0.40079999999999999</v>
+        <v>0.40110000000000001</v>
       </c>
       <c r="C14">
-        <v>15.968</v>
+        <v>15.967000000000001</v>
       </c>
       <c r="D14">
-        <v>0.3997</v>
+        <v>0.39979999999999999</v>
       </c>
       <c r="E14">
-        <v>16.004000000000001</v>
+        <v>22</v>
       </c>
       <c r="F14">
         <v>22</v>
       </c>
       <c r="G14">
-        <v>21</v>
-      </c>
-      <c r="H14">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>16.024999999999999</v>
+        <v>16.024000000000001</v>
       </c>
       <c r="B15">
-        <v>0.501</v>
+        <v>0.50139999999999996</v>
       </c>
       <c r="C15">
-        <v>15.954000000000001</v>
+        <v>15.952999999999999</v>
       </c>
       <c r="D15">
         <v>0.49990000000000001</v>
       </c>
       <c r="E15">
-        <v>15.997999999999999</v>
+        <v>23</v>
       </c>
       <c r="F15">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G15">
-        <v>22</v>
-      </c>
-      <c r="H15">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>16.024999999999999</v>
+        <v>16.024000000000001</v>
       </c>
       <c r="B16">
-        <v>0.60129999999999995</v>
+        <v>0.60160000000000002</v>
       </c>
       <c r="C16">
         <v>15.939</v>
       </c>
       <c r="D16">
-        <v>0.6</v>
+        <v>0.60009999999999997</v>
       </c>
       <c r="E16">
-        <v>15.992000000000001</v>
+        <v>23</v>
       </c>
       <c r="F16">
         <v>23</v>
       </c>
       <c r="G16">
-        <v>22</v>
-      </c>
-      <c r="H16">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>16.024999999999999</v>
+        <v>16.024000000000001</v>
       </c>
       <c r="B17">
-        <v>0.70150000000000001</v>
+        <v>0.70179999999999998</v>
       </c>
       <c r="C17">
         <v>15.923999999999999</v>
@@ -2714,354 +2582,312 @@
         <v>0.70020000000000004</v>
       </c>
       <c r="E17">
-        <v>15.986000000000001</v>
+        <v>24</v>
       </c>
       <c r="F17">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G17">
         <v>23</v>
       </c>
-      <c r="H17">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>16.024999999999999</v>
+        <v>16.024000000000001</v>
       </c>
       <c r="B18">
-        <v>0.80120000000000002</v>
+        <v>0.80149999999999999</v>
       </c>
       <c r="C18">
-        <v>15.91</v>
+        <v>15.909000000000001</v>
       </c>
       <c r="D18">
         <v>0.79959999999999998</v>
       </c>
       <c r="E18">
-        <v>15.978999999999999</v>
+        <v>25</v>
       </c>
       <c r="F18">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G18">
-        <v>23</v>
-      </c>
-      <c r="H18">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>16.024999999999999</v>
+        <v>16.024000000000001</v>
       </c>
       <c r="B19">
-        <v>0.90139999999999998</v>
+        <v>0.90169999999999995</v>
       </c>
       <c r="C19">
-        <v>15.895</v>
+        <v>15.894</v>
       </c>
       <c r="D19">
-        <v>0.89980000000000004</v>
+        <v>0.89970000000000006</v>
       </c>
       <c r="E19">
-        <v>15.973000000000001</v>
+        <v>26</v>
       </c>
       <c r="F19">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G19">
-        <v>24</v>
-      </c>
-      <c r="H19">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>16.024000000000001</v>
       </c>
       <c r="B20">
-        <v>1.0017</v>
+        <v>1.0019</v>
       </c>
       <c r="C20">
-        <v>15.88</v>
+        <v>15.878</v>
       </c>
       <c r="D20">
         <v>0.99990000000000001</v>
       </c>
       <c r="E20">
-        <v>15.965999999999999</v>
+        <v>27</v>
       </c>
       <c r="F20">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G20">
-        <v>25</v>
-      </c>
-      <c r="H20">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>16.024000000000001</v>
       </c>
       <c r="B21">
-        <v>1.1019000000000001</v>
+        <v>1.1021000000000001</v>
       </c>
       <c r="C21">
-        <v>15.864000000000001</v>
+        <v>15.862</v>
       </c>
       <c r="D21">
         <v>1.1000000000000001</v>
       </c>
       <c r="E21">
-        <v>15.96</v>
+        <v>28</v>
       </c>
       <c r="F21">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G21">
-        <v>26</v>
-      </c>
-      <c r="H21">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>16.024000000000001</v>
       </c>
       <c r="B22">
-        <v>1.2016</v>
+        <v>1.2018</v>
       </c>
       <c r="C22">
-        <v>15.848000000000001</v>
+        <v>15.846</v>
       </c>
       <c r="D22">
         <v>1.1997</v>
       </c>
       <c r="E22">
-        <v>15.952999999999999</v>
+        <v>29</v>
       </c>
       <c r="F22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G22">
-        <v>27</v>
-      </c>
-      <c r="H22">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>16.024000000000001</v>
       </c>
       <c r="B23">
-        <v>1.3019000000000001</v>
+        <v>1.3021</v>
       </c>
       <c r="C23">
-        <v>15.831</v>
+        <v>15.829000000000001</v>
       </c>
       <c r="D23">
         <v>1.2997000000000001</v>
       </c>
       <c r="E23">
-        <v>15.946</v>
+        <v>30</v>
       </c>
       <c r="F23">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G23">
-        <v>28</v>
-      </c>
-      <c r="H23">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>16.024000000000001</v>
+        <v>16.023</v>
       </c>
       <c r="B24">
-        <v>1.4020999999999999</v>
+        <v>1.4023000000000001</v>
       </c>
       <c r="C24">
-        <v>15.814</v>
+        <v>15.811999999999999</v>
       </c>
       <c r="D24">
         <v>1.3997999999999999</v>
       </c>
       <c r="E24">
-        <v>15.936999999999999</v>
+        <v>32</v>
       </c>
       <c r="F24">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G24">
-        <v>29</v>
-      </c>
-      <c r="H24">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>16.024000000000001</v>
+        <v>16.023</v>
       </c>
       <c r="B25">
-        <v>1.5023</v>
+        <v>1.5025999999999999</v>
       </c>
       <c r="C25">
-        <v>15.795999999999999</v>
+        <v>15.792999999999999</v>
       </c>
       <c r="D25">
         <v>1.5</v>
       </c>
       <c r="E25">
-        <v>15.93</v>
+        <v>34</v>
       </c>
       <c r="F25">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G25">
-        <v>31</v>
-      </c>
-      <c r="H25">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>16.024000000000001</v>
+        <v>16.023</v>
       </c>
       <c r="B26">
-        <v>1.6020000000000001</v>
+        <v>1.6023000000000001</v>
       </c>
       <c r="C26">
-        <v>15.776</v>
+        <v>15.775</v>
       </c>
       <c r="D26">
-        <v>1.5995999999999999</v>
+        <v>1.5996999999999999</v>
       </c>
       <c r="E26">
-        <v>15.920999999999999</v>
+        <v>35</v>
       </c>
       <c r="F26">
         <v>35</v>
       </c>
       <c r="G26">
-        <v>33</v>
-      </c>
-      <c r="H26">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>16.024000000000001</v>
+        <v>16.023</v>
       </c>
       <c r="B27">
-        <v>1.7023999999999999</v>
+        <v>1.7025999999999999</v>
       </c>
       <c r="C27">
-        <v>15.757</v>
+        <v>15.754</v>
       </c>
       <c r="D27">
         <v>1.7</v>
       </c>
       <c r="E27">
-        <v>15.913</v>
+        <v>38</v>
       </c>
       <c r="F27">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G27">
-        <v>35</v>
-      </c>
-      <c r="H27">
-        <v>22.4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>16.023</v>
       </c>
       <c r="B28">
-        <v>1.8026</v>
+        <v>1.8028999999999999</v>
       </c>
       <c r="C28">
-        <v>15.736000000000001</v>
+        <v>15.734</v>
       </c>
       <c r="D28">
         <v>1.8001</v>
       </c>
       <c r="E28">
-        <v>15.903</v>
+        <v>40</v>
       </c>
       <c r="F28">
         <v>40</v>
       </c>
       <c r="G28">
-        <v>37</v>
-      </c>
-      <c r="H28">
-        <v>22.4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>16.023</v>
       </c>
       <c r="B29">
-        <v>1.9029</v>
+        <v>1.9031</v>
       </c>
       <c r="C29">
-        <v>15.714</v>
+        <v>15.711</v>
       </c>
       <c r="D29">
         <v>1.9003000000000001</v>
       </c>
       <c r="E29">
-        <v>15.894</v>
+        <v>43</v>
       </c>
       <c r="F29">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G29">
-        <v>39</v>
-      </c>
-      <c r="H29">
-        <v>22.4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>16.023</v>
       </c>
       <c r="B30">
-        <v>2.0026000000000002</v>
+        <v>2.0028000000000001</v>
       </c>
       <c r="C30">
-        <v>15.689</v>
+        <v>15.688000000000001</v>
       </c>
       <c r="D30">
-        <v>1.9999</v>
+        <v>1.9990000000000001</v>
       </c>
       <c r="E30">
-        <v>15.882999999999999</v>
+        <v>46</v>
       </c>
       <c r="F30">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G30">
-        <v>43</v>
-      </c>
-      <c r="H30">
-        <v>22.4</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -3072,7 +2898,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B99306A9-EF66-EE48-BA84-1E1625B1BF9A}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
@@ -3080,7 +2906,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3102,762 +2928,672 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>24.056000000000001</v>
+        <v>24.050999999999998</v>
       </c>
       <c r="B2">
-        <v>1.26E-2</v>
+        <v>1.4500000000000001E-2</v>
       </c>
       <c r="C2">
-        <v>24.052</v>
+        <v>24.045999999999999</v>
       </c>
       <c r="D2">
         <v>1.01E-2</v>
       </c>
       <c r="E2">
-        <v>24.06</v>
+        <v>23</v>
       </c>
       <c r="F2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G2">
-        <v>21</v>
-      </c>
-      <c r="H2">
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>24.056000000000001</v>
+        <v>24.050999999999998</v>
       </c>
       <c r="B3">
-        <v>2.24E-2</v>
+        <v>2.4199999999999999E-2</v>
       </c>
       <c r="C3">
-        <v>24.050999999999998</v>
+        <v>24.044</v>
       </c>
       <c r="D3">
         <v>1.9900000000000001E-2</v>
       </c>
       <c r="E3">
-        <v>24.06</v>
+        <v>23</v>
       </c>
       <c r="F3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G3">
-        <v>21</v>
-      </c>
-      <c r="H3">
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>24.056000000000001</v>
+        <v>24.050999999999998</v>
       </c>
       <c r="B4">
-        <v>3.27E-2</v>
+        <v>3.4599999999999999E-2</v>
       </c>
       <c r="C4">
-        <v>24.048999999999999</v>
+        <v>24.042999999999999</v>
       </c>
       <c r="D4">
-        <v>3.0200000000000001E-2</v>
+        <v>3.0300000000000001E-2</v>
       </c>
       <c r="E4">
-        <v>24.06</v>
+        <v>23</v>
       </c>
       <c r="F4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G4">
-        <v>21</v>
-      </c>
-      <c r="H4">
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>24.056000000000001</v>
+        <v>24.050999999999998</v>
       </c>
       <c r="B5">
-        <v>4.2500000000000003E-2</v>
+        <v>4.4400000000000002E-2</v>
       </c>
       <c r="C5">
-        <v>24.047999999999998</v>
+        <v>24.041</v>
       </c>
       <c r="D5">
         <v>4.0099999999999997E-2</v>
       </c>
       <c r="E5">
-        <v>24.06</v>
+        <v>23</v>
       </c>
       <c r="F5">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G5">
-        <v>21</v>
-      </c>
-      <c r="H5">
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>24.056000000000001</v>
+        <v>24.050999999999998</v>
       </c>
       <c r="B6">
-        <v>5.2299999999999999E-2</v>
+        <v>5.4300000000000001E-2</v>
       </c>
       <c r="C6">
-        <v>24.045999999999999</v>
+        <v>24.04</v>
       </c>
       <c r="D6">
         <v>4.99E-2</v>
       </c>
       <c r="E6">
-        <v>24.06</v>
+        <v>23</v>
       </c>
       <c r="F6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G6">
-        <v>21</v>
-      </c>
-      <c r="H6">
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>24.056000000000001</v>
+        <v>24.050999999999998</v>
       </c>
       <c r="B7">
-        <v>6.2600000000000003E-2</v>
+        <v>6.4600000000000005E-2</v>
       </c>
       <c r="C7">
-        <v>24.045000000000002</v>
+        <v>24.038</v>
       </c>
       <c r="D7">
         <v>6.0199999999999997E-2</v>
       </c>
       <c r="E7">
-        <v>24.06</v>
+        <v>23</v>
       </c>
       <c r="F7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G7">
-        <v>21</v>
-      </c>
-      <c r="H7">
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>24.056000000000001</v>
+        <v>24.050999999999998</v>
       </c>
       <c r="B8">
-        <v>7.2499999999999995E-2</v>
+        <v>7.4399999999999994E-2</v>
       </c>
       <c r="C8">
-        <v>24.042999999999999</v>
+        <v>24.036999999999999</v>
       </c>
       <c r="D8">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0099999999999996E-2</v>
       </c>
       <c r="E8">
-        <v>24.06</v>
+        <v>23</v>
       </c>
       <c r="F8">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G8">
-        <v>21</v>
-      </c>
-      <c r="H8">
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>24.056000000000001</v>
+        <v>24.050999999999998</v>
       </c>
       <c r="B9">
-        <v>8.2400000000000001E-2</v>
+        <v>8.43E-2</v>
       </c>
       <c r="C9">
-        <v>24.042000000000002</v>
+        <v>24.035</v>
       </c>
       <c r="D9">
-        <v>7.9799999999999996E-2</v>
+        <v>7.9899999999999999E-2</v>
       </c>
       <c r="E9">
-        <v>24.06</v>
+        <v>23</v>
       </c>
       <c r="F9">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G9">
-        <v>21</v>
-      </c>
-      <c r="H9">
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>24.056000000000001</v>
+        <v>24.050999999999998</v>
       </c>
       <c r="B10">
-        <v>9.2600000000000002E-2</v>
+        <v>9.4600000000000004E-2</v>
       </c>
       <c r="C10">
-        <v>24.041</v>
+        <v>24.033999999999999</v>
       </c>
       <c r="D10">
         <v>9.0200000000000002E-2</v>
       </c>
       <c r="E10">
-        <v>24.06</v>
+        <v>23</v>
       </c>
       <c r="F10">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G10">
-        <v>21</v>
-      </c>
-      <c r="H10">
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>24.056000000000001</v>
+        <v>24.050999999999998</v>
       </c>
       <c r="B11">
-        <v>0.10249999999999999</v>
+        <v>0.10440000000000001</v>
       </c>
       <c r="C11">
-        <v>24.039000000000001</v>
+        <v>24.033000000000001</v>
       </c>
       <c r="D11">
         <v>0.1</v>
       </c>
       <c r="E11">
-        <v>24.06</v>
+        <v>23</v>
       </c>
       <c r="F11">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G11">
-        <v>21</v>
-      </c>
-      <c r="H11">
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>24.056000000000001</v>
+        <v>24.050999999999998</v>
       </c>
       <c r="B12">
-        <v>0.20269999999999999</v>
+        <v>0.2046</v>
       </c>
       <c r="C12">
-        <v>24.024999999999999</v>
+        <v>24.018999999999998</v>
       </c>
       <c r="D12">
-        <v>0.20019999999999999</v>
+        <v>0.20219999999999999</v>
       </c>
       <c r="E12">
-        <v>24.05</v>
+        <v>23</v>
       </c>
       <c r="F12">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G12">
-        <v>21</v>
-      </c>
-      <c r="H12">
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>24.056000000000001</v>
+        <v>24.050999999999998</v>
       </c>
       <c r="B13">
-        <v>0.3029</v>
+        <v>0.30480000000000002</v>
       </c>
       <c r="C13">
-        <v>24.012</v>
+        <v>24.004999999999999</v>
       </c>
       <c r="D13">
         <v>0.30020000000000002</v>
       </c>
       <c r="E13">
-        <v>24.05</v>
+        <v>23</v>
       </c>
       <c r="F13">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G13">
-        <v>21</v>
-      </c>
-      <c r="H13">
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>24.056000000000001</v>
+        <v>24.050999999999998</v>
       </c>
       <c r="B14">
-        <v>0.40260000000000001</v>
+        <v>0.40460000000000002</v>
       </c>
       <c r="C14">
-        <v>23.997</v>
+        <v>23.99</v>
       </c>
       <c r="D14">
         <v>0.39979999999999999</v>
       </c>
       <c r="E14">
-        <v>24.04</v>
+        <v>24</v>
       </c>
       <c r="F14">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G14">
-        <v>21</v>
-      </c>
-      <c r="H14">
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>24.056000000000001</v>
+        <v>24.050999999999998</v>
       </c>
       <c r="B15">
-        <v>0.50290000000000001</v>
+        <v>0.50480000000000003</v>
       </c>
       <c r="C15">
-        <v>23.983000000000001</v>
+        <v>23.975999999999999</v>
       </c>
       <c r="D15">
         <v>0.49990000000000001</v>
       </c>
       <c r="E15">
-        <v>24.04</v>
+        <v>24</v>
       </c>
       <c r="F15">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G15">
-        <v>22</v>
-      </c>
-      <c r="H15">
-        <v>22.6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>24.056000000000001</v>
+        <v>24.050999999999998</v>
       </c>
       <c r="B16">
-        <v>0.60309999999999997</v>
+        <v>0.60509999999999997</v>
       </c>
       <c r="C16">
-        <v>23.969000000000001</v>
+        <v>23.962</v>
       </c>
       <c r="D16">
         <v>0.60009999999999997</v>
       </c>
       <c r="E16">
-        <v>24.03</v>
+        <v>25</v>
       </c>
       <c r="F16">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G16">
-        <v>22</v>
-      </c>
-      <c r="H16">
-        <v>22.6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>24.056000000000001</v>
+        <v>24.05</v>
       </c>
       <c r="B17">
-        <v>0.70330000000000004</v>
+        <v>0.70520000000000005</v>
       </c>
       <c r="C17">
-        <v>23.954999999999998</v>
+        <v>23.946999999999999</v>
       </c>
       <c r="D17">
-        <v>0.70020000000000004</v>
+        <v>0.70030000000000003</v>
       </c>
       <c r="E17">
-        <v>24.02</v>
+        <v>25</v>
       </c>
       <c r="F17">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G17">
-        <v>23</v>
-      </c>
-      <c r="H17">
-        <v>22.7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>24.056000000000001</v>
+        <v>24.05</v>
       </c>
       <c r="B18">
-        <v>0.80300000000000005</v>
+        <v>0.80500000000000005</v>
       </c>
       <c r="C18">
-        <v>23.94</v>
+        <v>23.931999999999999</v>
       </c>
       <c r="D18">
-        <v>0.79959999999999998</v>
+        <v>0.79969999999999997</v>
       </c>
       <c r="E18">
-        <v>24.02</v>
+        <v>26</v>
       </c>
       <c r="F18">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G18">
-        <v>23</v>
-      </c>
-      <c r="H18">
-        <v>22.7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>24.055</v>
+        <v>24.05</v>
       </c>
       <c r="B19">
-        <v>0.90329999999999999</v>
+        <v>0.9052</v>
       </c>
       <c r="C19">
-        <v>23.925999999999998</v>
+        <v>23.917000000000002</v>
       </c>
       <c r="D19">
         <v>0.89980000000000004</v>
       </c>
       <c r="E19">
-        <v>24.01</v>
+        <v>27</v>
       </c>
       <c r="F19">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G19">
-        <v>24</v>
-      </c>
-      <c r="H19">
-        <v>22.7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>24.055</v>
+        <v>24.05</v>
       </c>
       <c r="B20">
-        <v>1.0035000000000001</v>
+        <v>1.0054000000000001</v>
       </c>
       <c r="C20">
-        <v>23.91</v>
+        <v>23.901</v>
       </c>
       <c r="D20">
         <v>0.99990000000000001</v>
       </c>
       <c r="E20">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F20">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G20">
-        <v>25</v>
-      </c>
-      <c r="H20">
-        <v>22.7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>24.055</v>
+        <v>24.05</v>
       </c>
       <c r="B21">
-        <v>1.1037999999999999</v>
+        <v>1.1055999999999999</v>
       </c>
       <c r="C21">
-        <v>23.893999999999998</v>
+        <v>23.885000000000002</v>
       </c>
       <c r="D21">
         <v>1.1001000000000001</v>
       </c>
       <c r="E21">
-        <v>23.99</v>
+        <v>29</v>
       </c>
       <c r="F21">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G21">
-        <v>26</v>
-      </c>
-      <c r="H21">
         <v>22.8</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>24.055</v>
+        <v>24.05</v>
       </c>
       <c r="B22">
-        <v>1.2034</v>
+        <v>1.2054</v>
       </c>
       <c r="C22">
-        <v>23.878</v>
+        <v>23.869</v>
       </c>
       <c r="D22">
         <v>1.1998</v>
       </c>
       <c r="E22">
-        <v>23.99</v>
+        <v>30</v>
       </c>
       <c r="F22">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G22">
-        <v>27</v>
-      </c>
-      <c r="H22">
         <v>22.8</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>24.055</v>
+        <v>24.05</v>
       </c>
       <c r="B23">
-        <v>1.3037000000000001</v>
+        <v>1.3056000000000001</v>
       </c>
       <c r="C23">
-        <v>23.861000000000001</v>
+        <v>23.852</v>
       </c>
       <c r="D23">
         <v>1.2998000000000001</v>
       </c>
       <c r="E23">
-        <v>23.98</v>
+        <v>32</v>
       </c>
       <c r="F23">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G23">
-        <v>29</v>
-      </c>
-      <c r="H23">
         <v>22.8</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>24.055</v>
+        <v>24.05</v>
       </c>
       <c r="B24">
-        <v>1.4037999999999999</v>
+        <v>1.4056999999999999</v>
       </c>
       <c r="C24">
-        <v>23.843</v>
+        <v>23.835000000000001</v>
       </c>
       <c r="D24">
-        <v>1.3998999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="E24">
-        <v>23.98</v>
+        <v>33</v>
       </c>
       <c r="F24">
         <v>33</v>
       </c>
       <c r="G24">
-        <v>30</v>
-      </c>
-      <c r="H24">
-        <v>22.9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>24.055</v>
+        <v>24.048999999999999</v>
       </c>
       <c r="B25">
-        <v>1.5041</v>
+        <v>1.506</v>
       </c>
       <c r="C25">
-        <v>23.826000000000001</v>
+        <v>23.815999999999999</v>
       </c>
       <c r="D25">
-        <v>1.5</v>
+        <v>1.5001</v>
       </c>
       <c r="E25">
-        <v>23.96</v>
+        <v>35</v>
       </c>
       <c r="F25">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G25">
-        <v>32</v>
-      </c>
-      <c r="H25">
-        <v>22.9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>24.055</v>
+        <v>24.048999999999999</v>
       </c>
       <c r="B26">
-        <v>1.6039000000000001</v>
+        <v>1.6056999999999999</v>
       </c>
       <c r="C26">
-        <v>23.806999999999999</v>
+        <v>23.797000000000001</v>
       </c>
       <c r="D26">
-        <v>1.5996999999999999</v>
+        <v>1.5998000000000001</v>
       </c>
       <c r="E26">
-        <v>23.96</v>
+        <v>37</v>
       </c>
       <c r="F26">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G26">
-        <v>34</v>
-      </c>
-      <c r="H26">
-        <v>22.9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>24.053999999999998</v>
+        <v>24.048999999999999</v>
       </c>
       <c r="B27">
-        <v>1.7041999999999999</v>
+        <v>1.7060999999999999</v>
       </c>
       <c r="C27">
-        <v>23.788</v>
+        <v>23.777999999999999</v>
       </c>
       <c r="D27">
         <v>1.7000999999999999</v>
       </c>
       <c r="E27">
-        <v>23.95</v>
+        <v>39</v>
       </c>
       <c r="F27">
         <v>39</v>
       </c>
       <c r="G27">
-        <v>35</v>
-      </c>
-      <c r="H27">
-        <v>22.9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>24.053999999999998</v>
+        <v>24.048999999999999</v>
       </c>
       <c r="B28">
-        <v>1.8044</v>
+        <v>1.8063</v>
       </c>
       <c r="C28">
-        <v>23.766999999999999</v>
+        <v>23.756</v>
       </c>
       <c r="D28">
-        <v>1.8001</v>
+        <v>1.8002</v>
       </c>
       <c r="E28">
-        <v>23.94</v>
+        <v>42</v>
       </c>
       <c r="F28">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G28">
-        <v>37</v>
-      </c>
-      <c r="H28">
-        <v>22.9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>24.053999999999998</v>
+        <v>24.048999999999999</v>
       </c>
       <c r="B29">
-        <v>1.9046000000000001</v>
+        <v>1.9065000000000001</v>
       </c>
       <c r="C29">
-        <v>23.745999999999999</v>
+        <v>23.733000000000001</v>
       </c>
       <c r="D29">
-        <v>1.9003000000000001</v>
+        <v>1.9004000000000001</v>
       </c>
       <c r="E29">
-        <v>23.93</v>
+        <v>44</v>
       </c>
       <c r="F29">
         <v>44</v>
       </c>
       <c r="G29">
-        <v>40</v>
-      </c>
-      <c r="H29">
-        <v>22.9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>24.053999999999998</v>
+        <v>24.048999999999999</v>
       </c>
       <c r="B30">
-        <v>2.0043000000000002</v>
+        <v>2.0062000000000002</v>
       </c>
       <c r="C30">
-        <v>23.722999999999999</v>
+        <v>23.71</v>
       </c>
       <c r="D30">
-        <v>1.9999</v>
+        <v>2</v>
       </c>
       <c r="E30">
-        <v>23.92</v>
+        <v>47</v>
       </c>
       <c r="F30">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G30">
-        <v>42</v>
-      </c>
-      <c r="H30">
-        <v>22.9</v>
+        <v>22.8</v>
       </c>
     </row>
   </sheetData>
@@ -3868,15 +3604,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ACFE5C5-6B8D-744D-A2E6-6323B97708D1}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3898,16 +3634,13 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>30.027999999999999</v>
+        <v>30.055</v>
       </c>
       <c r="B2">
-        <v>2.35E-2</v>
+        <v>2.3699999999999999E-2</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -3916,7 +3649,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>30.04</v>
+        <v>33</v>
+      </c>
+      <c r="F2">
+        <v>33</v>
+      </c>
+      <c r="G2">
+        <v>22.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove Va measurments for 10V tab
</commit_message>
<xml_diff>
--- a/data_analysis/xlsx/DMP4065S_Polarity_Overvoltage_Protection.xlsx
+++ b/data_analysis/xlsx/DMP4065S_Polarity_Overvoltage_Protection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelperry/Documents/GitHub/circuit_protection/data_analysis/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Dropbox\KiCAD\projects\circuit_protection\data_analysis\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DE72DD-6694-3F40-9F98-760DB3999A1E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82231023-F205-459D-AC98-AA54C135345D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="4" xr2:uid="{8AB7D094-8CEA-A04F-8AB1-5D165CB29E23}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005" xr2:uid="{8AB7D094-8CEA-A04F-8AB1-5D165CB29E23}"/>
   </bookViews>
   <sheets>
     <sheet name="Vin 10V" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="7">
   <si>
     <t>Vin</t>
   </si>
@@ -55,12 +55,6 @@
   </si>
   <si>
     <t>Tamb</t>
-  </si>
-  <si>
-    <t>Va*</t>
-  </si>
-  <si>
-    <t>* Keithley 177 drifted during data collection</t>
   </si>
 </sst>
 </file>
@@ -119,13 +113,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>63500</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>93536</xdr:rowOff>
@@ -687,15 +681,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEB92E55-A1A0-824A-A494-BDE0D38B5030}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -709,19 +703,16 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10.007999999999999</v>
       </c>
@@ -735,19 +726,16 @@
         <v>0.01</v>
       </c>
       <c r="E2">
-        <v>10.007999999999999</v>
+        <v>22</v>
       </c>
       <c r="F2">
         <v>22</v>
       </c>
       <c r="G2">
-        <v>22</v>
-      </c>
-      <c r="H2">
         <v>23.1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10.007999999999999</v>
       </c>
@@ -761,19 +749,16 @@
         <v>1.9800000000000002E-2</v>
       </c>
       <c r="E3">
-        <v>10.007999999999999</v>
+        <v>22</v>
       </c>
       <c r="F3">
         <v>22</v>
       </c>
       <c r="G3">
-        <v>22</v>
-      </c>
-      <c r="H3">
         <v>23.1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10.007999999999999</v>
       </c>
@@ -787,19 +772,16 @@
         <v>3.0200000000000001E-2</v>
       </c>
       <c r="E4">
-        <v>10.007</v>
+        <v>22</v>
       </c>
       <c r="F4">
         <v>22</v>
       </c>
       <c r="G4">
-        <v>22</v>
-      </c>
-      <c r="H4">
         <v>23.1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10.007999999999999</v>
       </c>
@@ -813,19 +795,16 @@
         <v>0.04</v>
       </c>
       <c r="E5">
-        <v>10.006</v>
+        <v>22</v>
       </c>
       <c r="F5">
         <v>22</v>
       </c>
       <c r="G5">
-        <v>22</v>
-      </c>
-      <c r="H5">
         <v>23.1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10.007999999999999</v>
       </c>
@@ -839,19 +818,16 @@
         <v>4.9799999999999997E-2</v>
       </c>
       <c r="E6">
-        <v>10.006</v>
+        <v>22</v>
       </c>
       <c r="F6">
         <v>22</v>
       </c>
       <c r="G6">
-        <v>22</v>
-      </c>
-      <c r="H6">
         <v>23.1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10.007999999999999</v>
       </c>
@@ -865,19 +841,16 @@
         <v>6.0100000000000001E-2</v>
       </c>
       <c r="E7">
-        <v>10.005000000000001</v>
+        <v>22</v>
       </c>
       <c r="F7">
         <v>22</v>
       </c>
       <c r="G7">
-        <v>22</v>
-      </c>
-      <c r="H7">
         <v>23.1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10.007999999999999</v>
       </c>
@@ -891,19 +864,16 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E8">
-        <v>10.004</v>
+        <v>22</v>
       </c>
       <c r="F8">
         <v>22</v>
       </c>
       <c r="G8">
-        <v>22</v>
-      </c>
-      <c r="H8">
         <v>23.1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10.007999999999999</v>
       </c>
@@ -917,19 +887,16 @@
         <v>7.9799999999999996E-2</v>
       </c>
       <c r="E9">
-        <v>10.004</v>
+        <v>22</v>
       </c>
       <c r="F9">
         <v>22</v>
       </c>
       <c r="G9">
-        <v>22</v>
-      </c>
-      <c r="H9">
         <v>23.1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10.007999999999999</v>
       </c>
@@ -943,19 +910,16 @@
         <v>9.01E-2</v>
       </c>
       <c r="E10">
-        <v>10.003</v>
+        <v>22</v>
       </c>
       <c r="F10">
         <v>22</v>
       </c>
       <c r="G10">
-        <v>22</v>
-      </c>
-      <c r="H10">
         <v>23.1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10.007999999999999</v>
       </c>
@@ -969,19 +933,16 @@
         <v>9.9900000000000003E-2</v>
       </c>
       <c r="E11">
-        <v>10.002000000000001</v>
+        <v>22</v>
       </c>
       <c r="F11">
         <v>22</v>
       </c>
       <c r="G11">
-        <v>22</v>
-      </c>
-      <c r="H11">
         <v>23.1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10.007</v>
       </c>
@@ -995,19 +956,16 @@
         <v>0.2001</v>
       </c>
       <c r="E12">
-        <v>9.9960000000000004</v>
+        <v>22</v>
       </c>
       <c r="F12">
         <v>22</v>
       </c>
       <c r="G12">
-        <v>22</v>
-      </c>
-      <c r="H12">
         <v>23.1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10.007</v>
       </c>
@@ -1021,19 +979,16 @@
         <v>0.30009999999999998</v>
       </c>
       <c r="E13">
-        <v>9.99</v>
+        <v>22</v>
       </c>
       <c r="F13">
         <v>22</v>
       </c>
       <c r="G13">
-        <v>22</v>
-      </c>
-      <c r="H13">
         <v>23.1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10.007</v>
       </c>
@@ -1047,19 +1002,16 @@
         <v>0.3997</v>
       </c>
       <c r="E14">
-        <v>9.9830000000000005</v>
+        <v>23</v>
       </c>
       <c r="F14">
         <v>23</v>
       </c>
       <c r="G14">
-        <v>23</v>
-      </c>
-      <c r="H14">
         <v>23.1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10.007</v>
       </c>
@@ -1073,19 +1025,16 @@
         <v>0.49980000000000002</v>
       </c>
       <c r="E15">
-        <v>9.9770000000000003</v>
+        <v>23</v>
       </c>
       <c r="F15">
         <v>23</v>
       </c>
       <c r="G15">
-        <v>23</v>
-      </c>
-      <c r="H15">
         <v>23.1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10.007</v>
       </c>
@@ -1099,19 +1048,16 @@
         <v>0.6</v>
       </c>
       <c r="E16">
-        <v>9.9700000000000006</v>
+        <v>23</v>
       </c>
       <c r="F16">
         <v>23</v>
       </c>
       <c r="G16">
-        <v>23</v>
-      </c>
-      <c r="H16">
         <v>23.1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10.007</v>
       </c>
@@ -1125,19 +1071,16 @@
         <v>0.70020000000000004</v>
       </c>
       <c r="E17">
-        <v>9.9640000000000004</v>
+        <v>24</v>
       </c>
       <c r="F17">
         <v>24</v>
       </c>
       <c r="G17">
-        <v>24</v>
-      </c>
-      <c r="H17">
         <v>23.1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10.007</v>
       </c>
@@ -1151,19 +1094,16 @@
         <v>0.79949999999999999</v>
       </c>
       <c r="E18">
-        <v>9.9570000000000007</v>
+        <v>25</v>
       </c>
       <c r="F18">
         <v>25</v>
       </c>
       <c r="G18">
-        <v>25</v>
-      </c>
-      <c r="H18">
         <v>23.1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10.007</v>
       </c>
@@ -1177,19 +1117,16 @@
         <v>0.89970000000000006</v>
       </c>
       <c r="E19">
-        <v>9.9499999999999993</v>
+        <v>26</v>
       </c>
       <c r="F19">
         <v>26</v>
       </c>
       <c r="G19">
-        <v>26</v>
-      </c>
-      <c r="H19">
         <v>23.1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10.007</v>
       </c>
@@ -1203,19 +1140,16 @@
         <v>0.99980000000000002</v>
       </c>
       <c r="E20">
-        <v>9.9420000000000002</v>
+        <v>27</v>
       </c>
       <c r="F20">
         <v>27</v>
       </c>
       <c r="G20">
-        <v>27</v>
-      </c>
-      <c r="H20">
         <v>23.2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10.006</v>
       </c>
@@ -1229,19 +1163,16 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="E21">
-        <v>9.9350000000000005</v>
+        <v>28</v>
       </c>
       <c r="F21">
         <v>28</v>
       </c>
       <c r="G21">
-        <v>28</v>
-      </c>
-      <c r="H21">
         <v>23.2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10.006</v>
       </c>
@@ -1255,19 +1186,16 @@
         <v>1.1997</v>
       </c>
       <c r="E22">
-        <v>9.9280000000000008</v>
+        <v>30</v>
       </c>
       <c r="F22">
         <v>30</v>
       </c>
       <c r="G22">
-        <v>30</v>
-      </c>
-      <c r="H22">
         <v>23.2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>10.006</v>
       </c>
@@ -1281,19 +1209,16 @@
         <v>1.2997000000000001</v>
       </c>
       <c r="E23">
-        <v>9.92</v>
+        <v>31</v>
       </c>
       <c r="F23">
         <v>31</v>
       </c>
       <c r="G23">
-        <v>31</v>
-      </c>
-      <c r="H23">
         <v>23.1</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>10.006</v>
       </c>
@@ -1307,22 +1232,16 @@
         <v>1.3997999999999999</v>
       </c>
       <c r="E24">
-        <v>9.9120000000000008</v>
+        <v>33</v>
       </c>
       <c r="F24">
         <v>33</v>
       </c>
       <c r="G24">
-        <v>33</v>
-      </c>
-      <c r="H24">
         <v>23.1</v>
       </c>
-      <c r="J24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>10.006</v>
       </c>
@@ -1336,19 +1255,16 @@
         <v>1.5</v>
       </c>
       <c r="E25">
-        <v>9.9039999999999999</v>
+        <v>35</v>
       </c>
       <c r="F25">
         <v>35</v>
       </c>
       <c r="G25">
-        <v>35</v>
-      </c>
-      <c r="H25">
         <v>23.1</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>10.006</v>
       </c>
@@ -1362,19 +1278,16 @@
         <v>1.5996999999999999</v>
       </c>
       <c r="E26">
-        <v>10.022</v>
+        <v>36</v>
       </c>
       <c r="F26">
         <v>36</v>
       </c>
       <c r="G26">
-        <v>36</v>
-      </c>
-      <c r="H26">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>10.006</v>
       </c>
@@ -1388,19 +1301,16 @@
         <v>1.7</v>
       </c>
       <c r="E27">
-        <v>10.013</v>
+        <v>38</v>
       </c>
       <c r="F27">
         <v>38</v>
       </c>
       <c r="G27">
-        <v>38</v>
-      </c>
-      <c r="H27">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>10.006</v>
       </c>
@@ -1414,19 +1324,16 @@
         <v>1.8001</v>
       </c>
       <c r="E28">
-        <v>10.002000000000001</v>
+        <v>41</v>
       </c>
       <c r="F28">
         <v>41</v>
       </c>
       <c r="G28">
-        <v>41</v>
-      </c>
-      <c r="H28">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>10.006</v>
       </c>
@@ -1440,19 +1347,16 @@
         <v>1.9001999999999999</v>
       </c>
       <c r="E29">
-        <v>9.9920000000000009</v>
+        <v>44</v>
       </c>
       <c r="F29">
         <v>44</v>
       </c>
       <c r="G29">
-        <v>44</v>
-      </c>
-      <c r="H29">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>10.005000000000001</v>
       </c>
@@ -1466,15 +1370,12 @@
         <v>1.9998</v>
       </c>
       <c r="E30">
-        <v>9.98</v>
+        <v>47</v>
       </c>
       <c r="F30">
         <v>47</v>
       </c>
       <c r="G30">
-        <v>47</v>
-      </c>
-      <c r="H30">
         <v>23</v>
       </c>
     </row>
@@ -1492,9 +1393,9 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1517,7 +1418,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>12.013999999999999</v>
       </c>
@@ -1540,7 +1441,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>12.013999999999999</v>
       </c>
@@ -1563,7 +1464,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>12.013999999999999</v>
       </c>
@@ -1586,7 +1487,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>12.013999999999999</v>
       </c>
@@ -1609,7 +1510,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>12.013999999999999</v>
       </c>
@@ -1632,7 +1533,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>12.013999999999999</v>
       </c>
@@ -1655,7 +1556,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>12.013999999999999</v>
       </c>
@@ -1678,7 +1579,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>12.013999999999999</v>
       </c>
@@ -1701,7 +1602,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>12.013999999999999</v>
       </c>
@@ -1724,7 +1625,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>12.013999999999999</v>
       </c>
@@ -1747,7 +1648,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12.013999999999999</v>
       </c>
@@ -1770,7 +1671,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12.013999999999999</v>
       </c>
@@ -1793,7 +1694,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12.013999999999999</v>
       </c>
@@ -1816,7 +1717,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12.013999999999999</v>
       </c>
@@ -1839,7 +1740,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12.013999999999999</v>
       </c>
@@ -1862,7 +1763,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>12.013999999999999</v>
       </c>
@@ -1885,7 +1786,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12.013</v>
       </c>
@@ -1908,7 +1809,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>12.013</v>
       </c>
@@ -1931,7 +1832,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>12.013</v>
       </c>
@@ -1954,7 +1855,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>12.013</v>
       </c>
@@ -1977,7 +1878,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>12.013</v>
       </c>
@@ -2000,7 +1901,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>12.013</v>
       </c>
@@ -2023,7 +1924,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>12.013</v>
       </c>
@@ -2046,7 +1947,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>12.013</v>
       </c>
@@ -2069,7 +1970,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>12.012</v>
       </c>
@@ -2092,7 +1993,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>12.012</v>
       </c>
@@ -2115,7 +2016,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>12.012</v>
       </c>
@@ -2138,7 +2039,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>12.012</v>
       </c>
@@ -2161,7 +2062,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>12.012</v>
       </c>
@@ -2198,9 +2099,9 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2223,7 +2124,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>16.024999999999999</v>
       </c>
@@ -2246,7 +2147,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>16.024999999999999</v>
       </c>
@@ -2269,7 +2170,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>16.024999999999999</v>
       </c>
@@ -2292,7 +2193,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>16.016999999999999</v>
       </c>
@@ -2315,7 +2216,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>16.024999999999999</v>
       </c>
@@ -2338,7 +2239,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>16.024999999999999</v>
       </c>
@@ -2361,7 +2262,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>16.024999999999999</v>
       </c>
@@ -2384,7 +2285,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>16.024999999999999</v>
       </c>
@@ -2407,7 +2308,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>16.024999999999999</v>
       </c>
@@ -2430,7 +2331,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>16.024999999999999</v>
       </c>
@@ -2453,7 +2354,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>16.024999999999999</v>
       </c>
@@ -2476,7 +2377,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>16.024999999999999</v>
       </c>
@@ -2499,7 +2400,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>16.024000000000001</v>
       </c>
@@ -2522,7 +2423,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>16.024000000000001</v>
       </c>
@@ -2545,7 +2446,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16.024000000000001</v>
       </c>
@@ -2568,7 +2469,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16.024000000000001</v>
       </c>
@@ -2591,7 +2492,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16.024000000000001</v>
       </c>
@@ -2614,7 +2515,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16.024000000000001</v>
       </c>
@@ -2637,7 +2538,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16.024000000000001</v>
       </c>
@@ -2660,7 +2561,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>16.024000000000001</v>
       </c>
@@ -2683,7 +2584,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>16.024000000000001</v>
       </c>
@@ -2706,7 +2607,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>16.024000000000001</v>
       </c>
@@ -2729,7 +2630,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>16.023</v>
       </c>
@@ -2752,7 +2653,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>16.023</v>
       </c>
@@ -2775,7 +2676,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>16.023</v>
       </c>
@@ -2798,7 +2699,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>16.023</v>
       </c>
@@ -2821,7 +2722,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>16.023</v>
       </c>
@@ -2844,7 +2745,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>16.023</v>
       </c>
@@ -2867,7 +2768,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>16.023</v>
       </c>
@@ -2904,9 +2805,9 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2929,7 +2830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>24.050999999999998</v>
       </c>
@@ -2952,7 +2853,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>24.050999999999998</v>
       </c>
@@ -2975,7 +2876,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>24.050999999999998</v>
       </c>
@@ -2998,7 +2899,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>24.050999999999998</v>
       </c>
@@ -3021,7 +2922,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>24.050999999999998</v>
       </c>
@@ -3044,7 +2945,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>24.050999999999998</v>
       </c>
@@ -3067,7 +2968,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>24.050999999999998</v>
       </c>
@@ -3090,7 +2991,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>24.050999999999998</v>
       </c>
@@ -3113,7 +3014,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>24.050999999999998</v>
       </c>
@@ -3136,7 +3037,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>24.050999999999998</v>
       </c>
@@ -3159,7 +3060,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>24.050999999999998</v>
       </c>
@@ -3182,7 +3083,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>24.050999999999998</v>
       </c>
@@ -3205,7 +3106,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>24.050999999999998</v>
       </c>
@@ -3228,7 +3129,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>24.050999999999998</v>
       </c>
@@ -3251,7 +3152,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>24.050999999999998</v>
       </c>
@@ -3274,7 +3175,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>24.05</v>
       </c>
@@ -3297,7 +3198,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>24.05</v>
       </c>
@@ -3320,7 +3221,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>24.05</v>
       </c>
@@ -3343,7 +3244,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>24.05</v>
       </c>
@@ -3366,7 +3267,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>24.05</v>
       </c>
@@ -3389,7 +3290,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>24.05</v>
       </c>
@@ -3412,7 +3313,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>24.05</v>
       </c>
@@ -3435,7 +3336,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24.05</v>
       </c>
@@ -3458,7 +3359,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24.048999999999999</v>
       </c>
@@ -3481,7 +3382,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24.048999999999999</v>
       </c>
@@ -3504,7 +3405,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>24.048999999999999</v>
       </c>
@@ -3527,7 +3428,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>24.048999999999999</v>
       </c>
@@ -3550,7 +3451,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>24.048999999999999</v>
       </c>
@@ -3573,7 +3474,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>24.048999999999999</v>
       </c>
@@ -3606,13 +3507,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ACFE5C5-6B8D-744D-A2E6-6323B97708D1}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3635,7 +3536,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>30.055</v>
       </c>

</xml_diff>